<commit_message>
Concats original address and gmaps address in the spreadsheet.
</commit_message>
<xml_diff>
--- a/Geocodeonthefly/Resources/model.xlsx
+++ b/Geocodeonthefly/Resources/model.xlsx
@@ -12,52 +12,55 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="CABO FRIO" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
     <t>Enter with your data from here...</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Neighborhood</t>
-  </si>
-  <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,9 +87,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,59 +406,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds 'Custom Identifier' column, fixes IsNullOrEmpty check, and updates model.xlsx.
</commit_message>
<xml_diff>
--- a/Geocodeonthefly/Resources/model.xlsx
+++ b/Geocodeonthefly/Resources/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Source\Repos\geocodeonthefly\Geocodeonthefly\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpsouza\Source\Repos\geocodeonthefly\Geocodeonthefly\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Street</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Enter with your data from here...</t>
+  </si>
+  <si>
+    <t>Custom Identifier</t>
   </si>
 </sst>
 </file>
@@ -404,36 +407,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -450,10 +458,14 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>